<commit_message>
Update Peru Primera División_2023.xlsx
</commit_message>
<xml_diff>
--- a/Bases_de_Dados_(2022-2023)/Peru Primera División_2023.xlsx
+++ b/Bases_de_Dados_(2022-2023)/Peru Primera División_2023.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="284">
   <si>
     <t>Id_Jogo</t>
   </si>
@@ -661,6 +661,12 @@
     <t>['16', '32', '85']</t>
   </si>
   <si>
+    <t>['54', '57']</t>
+  </si>
+  <si>
+    <t>['77']</t>
+  </si>
+  <si>
     <t>['81']</t>
   </si>
   <si>
@@ -1221,7 +1227,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BK169"/>
+  <dimension ref="A1:BK172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1552,7 +1558,7 @@
         <v>0</v>
       </c>
       <c r="AS2">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT2">
         <v>1.22</v>
@@ -2611,7 +2617,7 @@
         <v>87</v>
       </c>
       <c r="P8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="Q8">
         <v>9</v>
@@ -2802,7 +2808,7 @@
         <v>88</v>
       </c>
       <c r="P9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="Q9">
         <v>6</v>
@@ -3375,7 +3381,7 @@
         <v>90</v>
       </c>
       <c r="P12" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="Q12">
         <v>2</v>
@@ -3465,7 +3471,7 @@
         <v>0.89</v>
       </c>
       <c r="AT12">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU12">
         <v>0</v>
@@ -3566,7 +3572,7 @@
         <v>91</v>
       </c>
       <c r="P13" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="Q13">
         <v>6</v>
@@ -3757,7 +3763,7 @@
         <v>92</v>
       </c>
       <c r="P14" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="Q14">
         <v>7</v>
@@ -4035,7 +4041,7 @@
         <v>0</v>
       </c>
       <c r="AS15">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT15">
         <v>0.5600000000000001</v>
@@ -4229,7 +4235,7 @@
         <v>1.67</v>
       </c>
       <c r="AT16">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU16">
         <v>0</v>
@@ -4420,7 +4426,7 @@
         <v>1.67</v>
       </c>
       <c r="AT17">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU17">
         <v>0</v>
@@ -4712,7 +4718,7 @@
         <v>84</v>
       </c>
       <c r="P19" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="Q19">
         <v>6</v>
@@ -5285,7 +5291,7 @@
         <v>99</v>
       </c>
       <c r="P22" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="Q22">
         <v>10</v>
@@ -5372,7 +5378,7 @@
         <v>0</v>
       </c>
       <c r="AS22">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT22">
         <v>0.67</v>
@@ -5858,7 +5864,7 @@
         <v>101</v>
       </c>
       <c r="P25" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="Q25">
         <v>6</v>
@@ -6049,7 +6055,7 @@
         <v>102</v>
       </c>
       <c r="P26" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="Q26">
         <v>1</v>
@@ -6136,7 +6142,7 @@
         <v>1</v>
       </c>
       <c r="AS26">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT26">
         <v>0.5600000000000001</v>
@@ -6622,7 +6628,7 @@
         <v>105</v>
       </c>
       <c r="P29" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="Q29">
         <v>10</v>
@@ -6709,7 +6715,7 @@
         <v>3</v>
       </c>
       <c r="AS29">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT29">
         <v>1.22</v>
@@ -7476,7 +7482,7 @@
         <v>1.67</v>
       </c>
       <c r="AT33">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU33">
         <v>0.97</v>
@@ -7577,7 +7583,7 @@
         <v>110</v>
       </c>
       <c r="P34" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="Q34">
         <v>2</v>
@@ -7768,7 +7774,7 @@
         <v>111</v>
       </c>
       <c r="P35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="Q35">
         <v>8</v>
@@ -8046,7 +8052,7 @@
         <v>0</v>
       </c>
       <c r="AS36">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT36">
         <v>0.11</v>
@@ -8723,7 +8729,7 @@
         <v>84</v>
       </c>
       <c r="P40" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="Q40">
         <v>5</v>
@@ -8914,7 +8920,7 @@
         <v>84</v>
       </c>
       <c r="P41" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Q41">
         <v>8</v>
@@ -9105,7 +9111,7 @@
         <v>115</v>
       </c>
       <c r="P42" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="Q42">
         <v>11</v>
@@ -9192,7 +9198,7 @@
         <v>0</v>
       </c>
       <c r="AS42">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT42">
         <v>0.44</v>
@@ -10251,7 +10257,7 @@
         <v>121</v>
       </c>
       <c r="P48" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="Q48">
         <v>7</v>
@@ -10341,7 +10347,7 @@
         <v>1.56</v>
       </c>
       <c r="AT48">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU48">
         <v>1.61</v>
@@ -10442,7 +10448,7 @@
         <v>122</v>
       </c>
       <c r="P49" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Q49">
         <v>5</v>
@@ -10532,7 +10538,7 @@
         <v>1.78</v>
       </c>
       <c r="AT49">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU49">
         <v>1.41</v>
@@ -10633,7 +10639,7 @@
         <v>123</v>
       </c>
       <c r="P50" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="Q50">
         <v>3</v>
@@ -10911,7 +10917,7 @@
         <v>0</v>
       </c>
       <c r="AS51">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT51">
         <v>0.11</v>
@@ -11206,7 +11212,7 @@
         <v>125</v>
       </c>
       <c r="P53" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="Q53">
         <v>5</v>
@@ -11397,7 +11403,7 @@
         <v>126</v>
       </c>
       <c r="P54" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="Q54">
         <v>3</v>
@@ -11970,7 +11976,7 @@
         <v>129</v>
       </c>
       <c r="P57" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="Q57">
         <v>3</v>
@@ -12057,7 +12063,7 @@
         <v>2</v>
       </c>
       <c r="AS57">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT57">
         <v>1.67</v>
@@ -12248,7 +12254,7 @@
         <v>2</v>
       </c>
       <c r="AS58">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT58">
         <v>1.33</v>
@@ -12734,7 +12740,7 @@
         <v>84</v>
       </c>
       <c r="P61" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="Q61">
         <v>10</v>
@@ -13116,7 +13122,7 @@
         <v>134</v>
       </c>
       <c r="P63" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="Q63">
         <v>3</v>
@@ -13498,7 +13504,7 @@
         <v>84</v>
       </c>
       <c r="P65" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="Q65">
         <v>4</v>
@@ -13689,7 +13695,7 @@
         <v>135</v>
       </c>
       <c r="P66" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="Q66">
         <v>10</v>
@@ -14161,7 +14167,7 @@
         <v>1.44</v>
       </c>
       <c r="AT68">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU68">
         <v>1.59</v>
@@ -14352,7 +14358,7 @@
         <v>1.56</v>
       </c>
       <c r="AT69">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU69">
         <v>1.78</v>
@@ -14543,7 +14549,7 @@
         <v>1.56</v>
       </c>
       <c r="AT70">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU70">
         <v>2.17</v>
@@ -14644,7 +14650,7 @@
         <v>138</v>
       </c>
       <c r="P71" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="Q71">
         <v>3</v>
@@ -15026,7 +15032,7 @@
         <v>140</v>
       </c>
       <c r="P73" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="Q73">
         <v>5</v>
@@ -15599,7 +15605,7 @@
         <v>142</v>
       </c>
       <c r="P76" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="Q76">
         <v>7</v>
@@ -15877,7 +15883,7 @@
         <v>0.25</v>
       </c>
       <c r="AS77">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT77">
         <v>0.22</v>
@@ -15981,7 +15987,7 @@
         <v>84</v>
       </c>
       <c r="P78" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="Q78">
         <v>5</v>
@@ -16554,7 +16560,7 @@
         <v>84</v>
       </c>
       <c r="P81" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="Q81">
         <v>4</v>
@@ -16641,7 +16647,7 @@
         <v>1.8</v>
       </c>
       <c r="AS81">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT81">
         <v>1.67</v>
@@ -16745,7 +16751,7 @@
         <v>146</v>
       </c>
       <c r="P82" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Q82">
         <v>10</v>
@@ -16832,7 +16838,7 @@
         <v>0.4</v>
       </c>
       <c r="AS82">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT82">
         <v>0.89</v>
@@ -16936,7 +16942,7 @@
         <v>147</v>
       </c>
       <c r="P83" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="Q83">
         <v>6</v>
@@ -17127,7 +17133,7 @@
         <v>148</v>
       </c>
       <c r="P84" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="Q84">
         <v>10</v>
@@ -17509,7 +17515,7 @@
         <v>150</v>
       </c>
       <c r="P86" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="Q86">
         <v>8</v>
@@ -17891,7 +17897,7 @@
         <v>152</v>
       </c>
       <c r="P88" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="Q88">
         <v>11</v>
@@ -17981,7 +17987,7 @@
         <v>2</v>
       </c>
       <c r="AT88">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU88">
         <v>1.62</v>
@@ -18273,7 +18279,7 @@
         <v>154</v>
       </c>
       <c r="P90" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="Q90">
         <v>19</v>
@@ -18464,7 +18470,7 @@
         <v>84</v>
       </c>
       <c r="P91" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="Q91">
         <v>5</v>
@@ -18655,7 +18661,7 @@
         <v>155</v>
       </c>
       <c r="P92" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="Q92">
         <v>5</v>
@@ -18745,7 +18751,7 @@
         <v>1.44</v>
       </c>
       <c r="AT92">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU92">
         <v>1.6</v>
@@ -18846,7 +18852,7 @@
         <v>156</v>
       </c>
       <c r="P93" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="Q93">
         <v>9</v>
@@ -19419,7 +19425,7 @@
         <v>84</v>
       </c>
       <c r="P96" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="Q96">
         <v>5</v>
@@ -19610,7 +19616,7 @@
         <v>159</v>
       </c>
       <c r="P97" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="Q97">
         <v>6</v>
@@ -19697,7 +19703,7 @@
         <v>0.5</v>
       </c>
       <c r="AS97">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT97">
         <v>0.78</v>
@@ -19992,7 +19998,7 @@
         <v>151</v>
       </c>
       <c r="P99" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="Q99">
         <v>5</v>
@@ -20183,7 +20189,7 @@
         <v>161</v>
       </c>
       <c r="P100" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="Q100">
         <v>6</v>
@@ -20270,7 +20276,7 @@
         <v>1.5</v>
       </c>
       <c r="AS100">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT100">
         <v>1.22</v>
@@ -20374,7 +20380,7 @@
         <v>162</v>
       </c>
       <c r="P101" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="Q101">
         <v>6</v>
@@ -20461,7 +20467,7 @@
         <v>0.5</v>
       </c>
       <c r="AS101">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT101">
         <v>0.89</v>
@@ -20565,7 +20571,7 @@
         <v>163</v>
       </c>
       <c r="P102" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Q102">
         <v>5</v>
@@ -20846,7 +20852,7 @@
         <v>2.67</v>
       </c>
       <c r="AT103">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU103">
         <v>1.79</v>
@@ -21037,7 +21043,7 @@
         <v>2.33</v>
       </c>
       <c r="AT104">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU104">
         <v>1.38</v>
@@ -21329,7 +21335,7 @@
         <v>84</v>
       </c>
       <c r="P106" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="Q106">
         <v>1</v>
@@ -21419,7 +21425,7 @@
         <v>1.44</v>
       </c>
       <c r="AT106">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU106">
         <v>1.45</v>
@@ -21902,7 +21908,7 @@
         <v>167</v>
       </c>
       <c r="P109" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Q109">
         <v>5</v>
@@ -22284,7 +22290,7 @@
         <v>169</v>
       </c>
       <c r="P111" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="Q111">
         <v>5</v>
@@ -22944,7 +22950,7 @@
         <v>1.6</v>
       </c>
       <c r="AS114">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT114">
         <v>1.22</v>
@@ -23048,7 +23054,7 @@
         <v>173</v>
       </c>
       <c r="P115" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Q115">
         <v>6</v>
@@ -23135,7 +23141,7 @@
         <v>1</v>
       </c>
       <c r="AS115">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT115">
         <v>0.78</v>
@@ -23326,7 +23332,7 @@
         <v>0.8</v>
       </c>
       <c r="AS116">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT116">
         <v>0.5600000000000001</v>
@@ -23621,7 +23627,7 @@
         <v>174</v>
       </c>
       <c r="P118" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="Q118">
         <v>7</v>
@@ -23711,7 +23717,7 @@
         <v>1.78</v>
       </c>
       <c r="AT118">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU118">
         <v>1.5</v>
@@ -24194,7 +24200,7 @@
         <v>177</v>
       </c>
       <c r="P121" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Q121">
         <v>6</v>
@@ -24385,7 +24391,7 @@
         <v>178</v>
       </c>
       <c r="P122" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="Q122">
         <v>7</v>
@@ -24666,7 +24672,7 @@
         <v>3</v>
       </c>
       <c r="AT123">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU123">
         <v>1.61</v>
@@ -24854,7 +24860,7 @@
         <v>0.4</v>
       </c>
       <c r="AS124">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT124">
         <v>0.5600000000000001</v>
@@ -25340,7 +25346,7 @@
         <v>182</v>
       </c>
       <c r="P127" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="Q127">
         <v>4</v>
@@ -25430,7 +25436,7 @@
         <v>1.67</v>
       </c>
       <c r="AT127">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU127">
         <v>1.58</v>
@@ -25722,7 +25728,7 @@
         <v>184</v>
       </c>
       <c r="P129" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="Q129">
         <v>1</v>
@@ -25809,10 +25815,10 @@
         <v>1.67</v>
       </c>
       <c r="AS129">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT129">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU129">
         <v>1.57</v>
@@ -25913,7 +25919,7 @@
         <v>144</v>
       </c>
       <c r="P130" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="Q130">
         <v>7</v>
@@ -26003,7 +26009,7 @@
         <v>2</v>
       </c>
       <c r="AT130">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU130">
         <v>1.39</v>
@@ -26104,7 +26110,7 @@
         <v>185</v>
       </c>
       <c r="P131" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="Q131">
         <v>8</v>
@@ -26958,7 +26964,7 @@
         <v>1.78</v>
       </c>
       <c r="AT135">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU135">
         <v>1.76</v>
@@ -27059,7 +27065,7 @@
         <v>187</v>
       </c>
       <c r="P136" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="Q136">
         <v>3</v>
@@ -27340,7 +27346,7 @@
         <v>2.67</v>
       </c>
       <c r="AT137">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU137">
         <v>1.87</v>
@@ -27632,7 +27638,7 @@
         <v>189</v>
       </c>
       <c r="P139" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="Q139">
         <v>10</v>
@@ -27823,7 +27829,7 @@
         <v>190</v>
       </c>
       <c r="P140" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="Q140">
         <v>7</v>
@@ -28205,7 +28211,7 @@
         <v>134</v>
       </c>
       <c r="P142" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="Q142">
         <v>6</v>
@@ -28396,7 +28402,7 @@
         <v>192</v>
       </c>
       <c r="P143" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="Q143">
         <v>4</v>
@@ -29160,7 +29166,7 @@
         <v>196</v>
       </c>
       <c r="P147" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="Q147">
         <v>1</v>
@@ -29247,7 +29253,7 @@
         <v>0.57</v>
       </c>
       <c r="AS147">
-        <v>2.13</v>
+        <v>2</v>
       </c>
       <c r="AT147">
         <v>0.5600000000000001</v>
@@ -29438,7 +29444,7 @@
         <v>0.29</v>
       </c>
       <c r="AS148">
-        <v>2.63</v>
+        <v>2.67</v>
       </c>
       <c r="AT148">
         <v>0.5600000000000001</v>
@@ -29542,7 +29548,7 @@
         <v>198</v>
       </c>
       <c r="P149" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="Q149">
         <v>9</v>
@@ -29823,7 +29829,7 @@
         <v>1.78</v>
       </c>
       <c r="AT150">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="AU150">
         <v>1.57</v>
@@ -29924,7 +29930,7 @@
         <v>199</v>
       </c>
       <c r="P151" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="Q151">
         <v>4</v>
@@ -30011,10 +30017,10 @@
         <v>1.43</v>
       </c>
       <c r="AS151">
-        <v>1.63</v>
+        <v>1.78</v>
       </c>
       <c r="AT151">
-        <v>1.63</v>
+        <v>1.56</v>
       </c>
       <c r="AU151">
         <v>2.15</v>
@@ -30115,7 +30121,7 @@
         <v>200</v>
       </c>
       <c r="P152" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="Q152">
         <v>2</v>
@@ -30306,7 +30312,7 @@
         <v>201</v>
       </c>
       <c r="P153" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="Q153">
         <v>11</v>
@@ -30497,7 +30503,7 @@
         <v>202</v>
       </c>
       <c r="P154" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="Q154">
         <v>2</v>
@@ -30587,7 +30593,7 @@
         <v>1.89</v>
       </c>
       <c r="AT154">
-        <v>0.88</v>
+        <v>0.78</v>
       </c>
       <c r="AU154">
         <v>1.65</v>
@@ -30688,7 +30694,7 @@
         <v>203</v>
       </c>
       <c r="P155" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="Q155">
         <v>6</v>
@@ -30879,7 +30885,7 @@
         <v>204</v>
       </c>
       <c r="P156" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Q156">
         <v>8</v>
@@ -31643,7 +31649,7 @@
         <v>208</v>
       </c>
       <c r="P160" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="Q160">
         <v>15</v>
@@ -32598,7 +32604,7 @@
         <v>211</v>
       </c>
       <c r="P165" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="Q165">
         <v>7</v>
@@ -32789,7 +32795,7 @@
         <v>84</v>
       </c>
       <c r="P166" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="Q166">
         <v>2</v>
@@ -32980,7 +32986,7 @@
         <v>212</v>
       </c>
       <c r="P167" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="Q167">
         <v>5</v>
@@ -33171,7 +33177,7 @@
         <v>213</v>
       </c>
       <c r="P168" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="Q168">
         <v>6</v>
@@ -33362,7 +33368,7 @@
         <v>214</v>
       </c>
       <c r="P169" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="Q169">
         <v>3</v>
@@ -33504,6 +33510,579 @@
       </c>
       <c r="BK169">
         <v>14</v>
+      </c>
+    </row>
+    <row r="170" spans="1:63">
+      <c r="A170" s="1">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>5053111</v>
+      </c>
+      <c r="C170" t="s">
+        <v>63</v>
+      </c>
+      <c r="D170" t="s">
+        <v>64</v>
+      </c>
+      <c r="E170" s="2">
+        <v>45088.625</v>
+      </c>
+      <c r="F170">
+        <v>19</v>
+      </c>
+      <c r="G170" t="s">
+        <v>78</v>
+      </c>
+      <c r="H170" t="s">
+        <v>70</v>
+      </c>
+      <c r="I170">
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+      <c r="K170">
+        <v>0</v>
+      </c>
+      <c r="L170">
+        <v>0</v>
+      </c>
+      <c r="M170">
+        <v>0</v>
+      </c>
+      <c r="N170">
+        <v>0</v>
+      </c>
+      <c r="O170" t="s">
+        <v>84</v>
+      </c>
+      <c r="P170" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q170">
+        <v>1</v>
+      </c>
+      <c r="R170">
+        <v>8</v>
+      </c>
+      <c r="S170">
+        <v>9</v>
+      </c>
+      <c r="T170">
+        <v>4</v>
+      </c>
+      <c r="U170">
+        <v>2.25</v>
+      </c>
+      <c r="V170">
+        <v>2.6</v>
+      </c>
+      <c r="W170">
+        <v>1.35</v>
+      </c>
+      <c r="X170">
+        <v>3.2</v>
+      </c>
+      <c r="Y170">
+        <v>2.6</v>
+      </c>
+      <c r="Z170">
+        <v>1.43</v>
+      </c>
+      <c r="AA170">
+        <v>6.5</v>
+      </c>
+      <c r="AB170">
+        <v>1.1</v>
+      </c>
+      <c r="AC170">
+        <v>3.55</v>
+      </c>
+      <c r="AD170">
+        <v>3.6</v>
+      </c>
+      <c r="AE170">
+        <v>1.97</v>
+      </c>
+      <c r="AF170">
+        <v>1.03</v>
+      </c>
+      <c r="AG170">
+        <v>13</v>
+      </c>
+      <c r="AH170">
+        <v>1.23</v>
+      </c>
+      <c r="AI170">
+        <v>3.75</v>
+      </c>
+      <c r="AJ170">
+        <v>1.67</v>
+      </c>
+      <c r="AK170">
+        <v>2</v>
+      </c>
+      <c r="AL170">
+        <v>1.7</v>
+      </c>
+      <c r="AM170">
+        <v>2.15</v>
+      </c>
+      <c r="AN170">
+        <v>1.87</v>
+      </c>
+      <c r="AO170">
+        <v>1.22</v>
+      </c>
+      <c r="AP170">
+        <v>1.28</v>
+      </c>
+      <c r="AQ170">
+        <v>2.13</v>
+      </c>
+      <c r="AR170">
+        <v>1.63</v>
+      </c>
+      <c r="AS170">
+        <v>2</v>
+      </c>
+      <c r="AT170">
+        <v>1.56</v>
+      </c>
+      <c r="AU170">
+        <v>1.57</v>
+      </c>
+      <c r="AV170">
+        <v>1.36</v>
+      </c>
+      <c r="AW170">
+        <v>2.93</v>
+      </c>
+      <c r="AX170">
+        <v>2.63</v>
+      </c>
+      <c r="AY170">
+        <v>8.5</v>
+      </c>
+      <c r="AZ170">
+        <v>1.62</v>
+      </c>
+      <c r="BA170">
+        <v>1.2</v>
+      </c>
+      <c r="BB170">
+        <v>1.32</v>
+      </c>
+      <c r="BC170">
+        <v>1.56</v>
+      </c>
+      <c r="BD170">
+        <v>1.9</v>
+      </c>
+      <c r="BE170">
+        <v>2.62</v>
+      </c>
+      <c r="BF170">
+        <v>2</v>
+      </c>
+      <c r="BG170">
+        <v>8</v>
+      </c>
+      <c r="BH170">
+        <v>5</v>
+      </c>
+      <c r="BI170">
+        <v>9</v>
+      </c>
+      <c r="BJ170">
+        <v>7</v>
+      </c>
+      <c r="BK170">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="171" spans="1:63">
+      <c r="A171" s="1">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>5053109</v>
+      </c>
+      <c r="C171" t="s">
+        <v>63</v>
+      </c>
+      <c r="D171" t="s">
+        <v>64</v>
+      </c>
+      <c r="E171" s="2">
+        <v>45088.72916666666</v>
+      </c>
+      <c r="F171">
+        <v>19</v>
+      </c>
+      <c r="G171" t="s">
+        <v>65</v>
+      </c>
+      <c r="H171" t="s">
+        <v>72</v>
+      </c>
+      <c r="I171">
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+      <c r="K171">
+        <v>0</v>
+      </c>
+      <c r="L171">
+        <v>2</v>
+      </c>
+      <c r="M171">
+        <v>0</v>
+      </c>
+      <c r="N171">
+        <v>2</v>
+      </c>
+      <c r="O171" t="s">
+        <v>215</v>
+      </c>
+      <c r="P171" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q171">
+        <v>7</v>
+      </c>
+      <c r="R171">
+        <v>3</v>
+      </c>
+      <c r="S171">
+        <v>10</v>
+      </c>
+      <c r="T171">
+        <v>2.1</v>
+      </c>
+      <c r="U171">
+        <v>2.25</v>
+      </c>
+      <c r="V171">
+        <v>6</v>
+      </c>
+      <c r="W171">
+        <v>1.4</v>
+      </c>
+      <c r="X171">
+        <v>3.1</v>
+      </c>
+      <c r="Y171">
+        <v>2.63</v>
+      </c>
+      <c r="Z171">
+        <v>1.4</v>
+      </c>
+      <c r="AA171">
+        <v>6.5</v>
+      </c>
+      <c r="AB171">
+        <v>1.08</v>
+      </c>
+      <c r="AC171">
+        <v>1.53</v>
+      </c>
+      <c r="AD171">
+        <v>3.7</v>
+      </c>
+      <c r="AE171">
+        <v>5.25</v>
+      </c>
+      <c r="AF171">
+        <v>1.03</v>
+      </c>
+      <c r="AG171">
+        <v>10</v>
+      </c>
+      <c r="AH171">
+        <v>1.29</v>
+      </c>
+      <c r="AI171">
+        <v>3.24</v>
+      </c>
+      <c r="AJ171">
+        <v>1.85</v>
+      </c>
+      <c r="AK171">
+        <v>1.95</v>
+      </c>
+      <c r="AL171">
+        <v>1.95</v>
+      </c>
+      <c r="AM171">
+        <v>1.8</v>
+      </c>
+      <c r="AN171">
+        <v>1.11</v>
+      </c>
+      <c r="AO171">
+        <v>1.18</v>
+      </c>
+      <c r="AP171">
+        <v>2.45</v>
+      </c>
+      <c r="AQ171">
+        <v>2.63</v>
+      </c>
+      <c r="AR171">
+        <v>0.88</v>
+      </c>
+      <c r="AS171">
+        <v>2.67</v>
+      </c>
+      <c r="AT171">
+        <v>0.78</v>
+      </c>
+      <c r="AU171">
+        <v>1.62</v>
+      </c>
+      <c r="AV171">
+        <v>1.19</v>
+      </c>
+      <c r="AW171">
+        <v>2.81</v>
+      </c>
+      <c r="AX171">
+        <v>1.33</v>
+      </c>
+      <c r="AY171">
+        <v>9.5</v>
+      </c>
+      <c r="AZ171">
+        <v>3.74</v>
+      </c>
+      <c r="BA171">
+        <v>1.17</v>
+      </c>
+      <c r="BB171">
+        <v>1.28</v>
+      </c>
+      <c r="BC171">
+        <v>1.51</v>
+      </c>
+      <c r="BD171">
+        <v>1.95</v>
+      </c>
+      <c r="BE171">
+        <v>2.45</v>
+      </c>
+      <c r="BF171">
+        <v>9</v>
+      </c>
+      <c r="BG171">
+        <v>0</v>
+      </c>
+      <c r="BH171">
+        <v>5</v>
+      </c>
+      <c r="BI171">
+        <v>4</v>
+      </c>
+      <c r="BJ171">
+        <v>14</v>
+      </c>
+      <c r="BK171">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="172" spans="1:63">
+      <c r="A172" s="1">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>5053112</v>
+      </c>
+      <c r="C172" t="s">
+        <v>63</v>
+      </c>
+      <c r="D172" t="s">
+        <v>64</v>
+      </c>
+      <c r="E172" s="2">
+        <v>45088.83333333334</v>
+      </c>
+      <c r="F172">
+        <v>19</v>
+      </c>
+      <c r="G172" t="s">
+        <v>83</v>
+      </c>
+      <c r="H172" t="s">
+        <v>67</v>
+      </c>
+      <c r="I172">
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+      <c r="K172">
+        <v>0</v>
+      </c>
+      <c r="L172">
+        <v>1</v>
+      </c>
+      <c r="M172">
+        <v>0</v>
+      </c>
+      <c r="N172">
+        <v>1</v>
+      </c>
+      <c r="O172" t="s">
+        <v>216</v>
+      </c>
+      <c r="P172" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q172">
+        <v>2</v>
+      </c>
+      <c r="R172">
+        <v>1</v>
+      </c>
+      <c r="S172">
+        <v>3</v>
+      </c>
+      <c r="T172">
+        <v>3</v>
+      </c>
+      <c r="U172">
+        <v>2.2</v>
+      </c>
+      <c r="V172">
+        <v>3.4</v>
+      </c>
+      <c r="W172">
+        <v>1.4</v>
+      </c>
+      <c r="X172">
+        <v>3</v>
+      </c>
+      <c r="Y172">
+        <v>2.8</v>
+      </c>
+      <c r="Z172">
+        <v>1.4</v>
+      </c>
+      <c r="AA172">
+        <v>7</v>
+      </c>
+      <c r="AB172">
+        <v>1.08</v>
+      </c>
+      <c r="AC172">
+        <v>2.44</v>
+      </c>
+      <c r="AD172">
+        <v>3.2</v>
+      </c>
+      <c r="AE172">
+        <v>2.58</v>
+      </c>
+      <c r="AF172">
+        <v>1.04</v>
+      </c>
+      <c r="AG172">
+        <v>12</v>
+      </c>
+      <c r="AH172">
+        <v>1.3</v>
+      </c>
+      <c r="AI172">
+        <v>3.6</v>
+      </c>
+      <c r="AJ172">
+        <v>1.81</v>
+      </c>
+      <c r="AK172">
+        <v>1.9</v>
+      </c>
+      <c r="AL172">
+        <v>1.72</v>
+      </c>
+      <c r="AM172">
+        <v>2.05</v>
+      </c>
+      <c r="AN172">
+        <v>1.38</v>
+      </c>
+      <c r="AO172">
+        <v>1.25</v>
+      </c>
+      <c r="AP172">
+        <v>1.65</v>
+      </c>
+      <c r="AQ172">
+        <v>1.63</v>
+      </c>
+      <c r="AR172">
+        <v>1.25</v>
+      </c>
+      <c r="AS172">
+        <v>1.78</v>
+      </c>
+      <c r="AT172">
+        <v>1.11</v>
+      </c>
+      <c r="AU172">
+        <v>2.09</v>
+      </c>
+      <c r="AV172">
+        <v>1.33</v>
+      </c>
+      <c r="AW172">
+        <v>3.42</v>
+      </c>
+      <c r="AX172">
+        <v>2.1</v>
+      </c>
+      <c r="AY172">
+        <v>8</v>
+      </c>
+      <c r="AZ172">
+        <v>1.95</v>
+      </c>
+      <c r="BA172">
+        <v>1.18</v>
+      </c>
+      <c r="BB172">
+        <v>1.35</v>
+      </c>
+      <c r="BC172">
+        <v>1.59</v>
+      </c>
+      <c r="BD172">
+        <v>2</v>
+      </c>
+      <c r="BE172">
+        <v>2.5</v>
+      </c>
+      <c r="BF172">
+        <v>6</v>
+      </c>
+      <c r="BG172">
+        <v>4</v>
+      </c>
+      <c r="BH172">
+        <v>7</v>
+      </c>
+      <c r="BI172">
+        <v>7</v>
+      </c>
+      <c r="BJ172">
+        <v>13</v>
+      </c>
+      <c r="BK172">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>